<commit_message>
voronoi treemap for remit group; init draft
</commit_message>
<xml_diff>
--- a/data/avg_spending_byCat_normalized.xlsx
+++ b/data/avg_spending_byCat_normalized.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/runlanlana/Documents/2023_Spring/MIT6.C85_Interactive Data Visualization and Society/Final Project/MigrationMDT/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C21B26C1-FB82-AF44-A9F8-E6B559D4E2B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEC7A12F-789F-784C-B4B4-57EBE85442D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1180" yWindow="1500" windowWidth="27240" windowHeight="15380" activeTab="1" xr2:uid="{90FB2B7F-F2DC-A947-B420-8E21EAE8B889}"/>
+    <workbookView xWindow="1180" yWindow="1500" windowWidth="27240" windowHeight="15380" xr2:uid="{90FB2B7F-F2DC-A947-B420-8E21EAE8B889}"/>
   </bookViews>
   <sheets>
     <sheet name="remittances" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="23">
   <si>
     <t>Food</t>
   </si>
@@ -92,6 +92,21 @@
   </si>
   <si>
     <t>Housing contruction/repair</t>
+  </si>
+  <si>
+    <t>Utilities</t>
+  </si>
+  <si>
+    <t>Housing</t>
+  </si>
+  <si>
+    <t>Personal Spending</t>
+  </si>
+  <si>
+    <t>Savings &amp; Debt</t>
+  </si>
+  <si>
+    <t>Productive Supplies</t>
   </si>
 </sst>
 </file>
@@ -443,10 +458,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44DB7E41-2D86-5346-BF0E-2692AD0D4BF7}">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView zoomScale="135" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B18"/>
+    <sheetView tabSelected="1" zoomScale="135" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -454,7 +469,7 @@
     <col min="1" max="1" width="31.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -465,8 +480,11 @@
         <f>B1/$B$20*100</f>
         <v>33.772619365877986</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -477,8 +495,11 @@
         <f t="shared" ref="C2:C18" si="0">B2/$B$20*100</f>
         <v>1.8707115997244377</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -489,8 +510,11 @@
         <f t="shared" si="0"/>
         <v>1.8070944756038538</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -501,8 +525,11 @@
         <f t="shared" si="0"/>
         <v>2.4253115880761116</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -513,8 +540,11 @@
         <f t="shared" si="0"/>
         <v>6.0054365956631566</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -525,8 +555,11 @@
         <f t="shared" si="0"/>
         <v>6.5081871961263653</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -537,8 +570,11 @@
         <f t="shared" si="0"/>
         <v>5.3850413165736954</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -549,8 +585,11 @@
         <f t="shared" si="0"/>
         <v>3.8770299847662546</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -561,8 +600,11 @@
         <f t="shared" si="0"/>
         <v>3.1765582159453492</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -573,8 +615,11 @@
         <f t="shared" si="0"/>
         <v>0.72671473342956294</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -585,8 +630,11 @@
         <f t="shared" si="0"/>
         <v>9.8750630926947878</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -597,8 +645,11 @@
         <f t="shared" si="0"/>
         <v>1.5551794828781513</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -609,8 +660,11 @@
         <f t="shared" si="0"/>
         <v>1.3031424779730221</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -621,8 +675,11 @@
         <f t="shared" si="0"/>
         <v>6.3260099378507935</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -633,8 +690,11 @@
         <f t="shared" si="0"/>
         <v>1.2722053057705995</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D15" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -645,8 +705,11 @@
         <f t="shared" si="0"/>
         <v>2.7159657995495663</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -657,8 +720,11 @@
         <f t="shared" si="0"/>
         <v>2.3580583544484943</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D17" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -669,8 +735,11 @@
         <f t="shared" si="0"/>
         <v>9.0396704770477996</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D18" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B20">
         <f>SUM(B1:B18)</f>
         <v>205.2129716367194</v>
@@ -685,7 +754,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FE52A77-9E88-B54C-829A-60F01E33428B}">
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+    <sheetView zoomScale="125" workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
fixed labels, added no remit group; changed ratio to amount
</commit_message>
<xml_diff>
--- a/data/avg_spending_byCat_normalized.xlsx
+++ b/data/avg_spending_byCat_normalized.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/runlanlana/Documents/2023_Spring/MIT6.C85_Interactive Data Visualization and Society/Final Project/MigrationMDT/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEC7A12F-789F-784C-B4B4-57EBE85442D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07E8CBD2-3E7E-2043-AF58-2F30CBD495F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1180" yWindow="1500" windowWidth="27240" windowHeight="15380" xr2:uid="{90FB2B7F-F2DC-A947-B420-8E21EAE8B889}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="No remittances" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="29">
   <si>
     <t>Food</t>
   </si>
@@ -107,6 +107,24 @@
   </si>
   <si>
     <t>Productive Supplies</t>
+  </si>
+  <si>
+    <t>category</t>
+  </si>
+  <si>
+    <t>spending</t>
+  </si>
+  <si>
+    <t>exp_remit</t>
+  </si>
+  <si>
+    <t>exp_remit_normalized</t>
+  </si>
+  <si>
+    <t>exp_noRemit</t>
+  </si>
+  <si>
+    <t>noRemit_remit_ratio</t>
   </si>
 </sst>
 </file>
@@ -458,291 +476,442 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44DB7E41-2D86-5346-BF0E-2692AD0D4BF7}">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="135" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="31.33203125" customWidth="1"/>
+    <col min="2" max="2" width="31.33203125" customWidth="1"/>
+    <col min="4" max="4" width="22.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B1">
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2">
         <v>69.3057958002764</v>
       </c>
-      <c r="C1">
-        <f>B1/$B$20*100</f>
+      <c r="D2">
+        <f>C2/$C$21*100</f>
         <v>33.772619365877986</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E2">
+        <v>45.166598522649998</v>
+      </c>
+      <c r="F2">
+        <f>E2/C2</f>
+        <v>0.65170016448277868</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="B3" t="s">
         <v>1</v>
       </c>
-      <c r="B2">
+      <c r="C3">
         <v>3.83894286454733</v>
       </c>
-      <c r="C2">
-        <f t="shared" ref="C2:C18" si="0">B2/$B$20*100</f>
+      <c r="D3">
+        <f t="shared" ref="D3:D19" si="0">C3/$C$21*100</f>
         <v>1.8707115997244377</v>
       </c>
-      <c r="D2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="E3">
+        <v>2.1422585671007899</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F19" si="1">E3/C3</f>
+        <v>0.55803345938918913</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s">
         <v>2</v>
       </c>
-      <c r="B3">
+      <c r="C4">
         <v>3.7083922736696602</v>
       </c>
-      <c r="C3">
+      <c r="D4">
         <f t="shared" si="0"/>
         <v>1.8070944756038538</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E4">
+        <v>2.1143398278595602</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="1"/>
+        <v>0.57014999272644462</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>4.9770539813407</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>2.4253115880761116</v>
+      </c>
+      <c r="E5">
+        <v>3.94235867412231</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="1"/>
+        <v>0.79210687464963603</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>4.9770539813407</v>
-      </c>
-      <c r="C4">
-        <f t="shared" si="0"/>
-        <v>2.4253115880761116</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <v>12.323934897719401</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>6.0054365956631566</v>
+      </c>
+      <c r="E6">
+        <v>7.8301082151755299</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="1"/>
+        <v>0.63535780415592158</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <v>12.323934897719401</v>
-      </c>
-      <c r="C5">
-        <f t="shared" si="0"/>
-        <v>6.0054365956631566</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7">
+        <v>13.355644344851401</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>6.5081871961263653</v>
+      </c>
+      <c r="E7">
+        <v>8.7274658819365794</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="1"/>
+        <v>0.65346647878512998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8">
+        <v>11.050803309606</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>5.3850413165736954</v>
+      </c>
+      <c r="E8">
+        <v>8.4198711172140399</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="1"/>
+        <v>0.76192389650940573</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6">
-        <v>13.355644344851401</v>
-      </c>
-      <c r="C6">
-        <f t="shared" si="0"/>
-        <v>6.5081871961263653</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9">
+        <v>7.9561684429854802</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>3.8770299847662546</v>
+      </c>
+      <c r="E9">
+        <v>5.0862148338052098</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="1"/>
+        <v>0.63927943082822081</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10">
+        <v>6.51870951071181</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>3.1765582159453492</v>
+      </c>
+      <c r="E10">
+        <v>4.7786268244620604</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="1"/>
+        <v>0.73306331822420145</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11">
+        <v>1.4913128997926699</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>0.72671473342956294</v>
+      </c>
+      <c r="E11">
+        <v>0.67826332163080405</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="1"/>
+        <v>0.45480953173884553</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12">
+        <v>20.2649104235199</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>9.8750630926947878</v>
+      </c>
+      <c r="E12">
+        <v>8.1229291259909395</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="1"/>
+        <v>0.40083715921898622</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13">
+        <v>3.19143003109882</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>1.5551794828781513</v>
+      </c>
+      <c r="E13">
+        <v>2.3754505915439701</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="1"/>
+        <v>0.74432168914763719</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14">
+        <v>2.6742174037088202</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>1.3031424779730221</v>
+      </c>
+      <c r="E14">
+        <v>1.7552700438372899</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="1"/>
+        <v>0.65636774385019703</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15">
+        <v>12.981792979497801</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>6.3260099378507935</v>
+      </c>
+      <c r="E15">
+        <v>11.1303832019158</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="1"/>
+        <v>0.85738412401846653</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16">
+        <v>2.6107303132918598</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="0"/>
+        <v>1.2722053057705995</v>
+      </c>
+      <c r="E16">
+        <v>0.79759144842393304</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="1"/>
+        <v>0.30550510880545645</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17">
+        <v>5.5735141258926504</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="0"/>
+        <v>2.7159657995495663</v>
+      </c>
+      <c r="E17">
+        <v>5.5518454757455604</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="1"/>
+        <v>0.99611221041919951</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18">
+        <v>4.8390416220916803</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="0"/>
+        <v>2.3580583544484943</v>
+      </c>
+      <c r="E18">
+        <v>1.65591512835032</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="1"/>
+        <v>0.34219898435892127</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7">
-        <v>11.050803309606</v>
-      </c>
-      <c r="C7">
-        <f t="shared" si="0"/>
-        <v>5.3850413165736954</v>
-      </c>
-      <c r="D7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8">
-        <v>7.9561684429854802</v>
-      </c>
-      <c r="C8">
-        <f t="shared" si="0"/>
-        <v>3.8770299847662546</v>
-      </c>
-      <c r="D8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9">
-        <v>6.51870951071181</v>
-      </c>
-      <c r="C9">
-        <f t="shared" si="0"/>
-        <v>3.1765582159453492</v>
-      </c>
-      <c r="D9" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10">
-        <v>1.4913128997926699</v>
-      </c>
-      <c r="C10">
-        <f t="shared" si="0"/>
-        <v>0.72671473342956294</v>
-      </c>
-      <c r="D10" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11">
-        <v>20.2649104235199</v>
-      </c>
-      <c r="C11">
-        <f t="shared" si="0"/>
-        <v>9.8750630926947878</v>
-      </c>
-      <c r="D11" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12">
-        <v>3.19143003109882</v>
-      </c>
-      <c r="C12">
-        <f t="shared" si="0"/>
-        <v>1.5551794828781513</v>
-      </c>
-      <c r="D12" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13">
-        <v>2.6742174037088202</v>
-      </c>
-      <c r="C13">
-        <f t="shared" si="0"/>
-        <v>1.3031424779730221</v>
-      </c>
-      <c r="D13" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14">
-        <v>12.981792979497801</v>
-      </c>
-      <c r="C14">
-        <f t="shared" si="0"/>
-        <v>6.3260099378507935</v>
-      </c>
-      <c r="D14" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15">
-        <v>2.6107303132918598</v>
-      </c>
-      <c r="C15">
-        <f t="shared" si="0"/>
-        <v>1.2722053057705995</v>
-      </c>
-      <c r="D15" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>15</v>
-      </c>
-      <c r="B16">
-        <v>5.5735141258926504</v>
-      </c>
-      <c r="C16">
-        <f t="shared" si="0"/>
-        <v>2.7159657995495663</v>
-      </c>
-      <c r="D16" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>16</v>
-      </c>
-      <c r="B17">
-        <v>4.8390416220916803</v>
-      </c>
-      <c r="C17">
-        <f t="shared" si="0"/>
-        <v>2.3580583544484943</v>
-      </c>
-      <c r="D17" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+      <c r="B19" t="s">
         <v>17</v>
       </c>
-      <c r="B18">
+      <c r="C19">
         <v>18.550576412117</v>
       </c>
-      <c r="C18">
+      <c r="D19">
         <f t="shared" si="0"/>
         <v>9.0396704770477996</v>
       </c>
-      <c r="D18" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B20">
-        <f>SUM(B1:B18)</f>
+      <c r="E19">
+        <v>6.7641167033786296</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="1"/>
+        <v>0.36463107954750101</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C21">
+        <f>SUM(C2:C19)</f>
         <v>205.2129716367194</v>
+      </c>
+      <c r="E21">
+        <f>SUM(E2:E19)</f>
+        <v>127.03960750514334</v>
       </c>
     </row>
   </sheetData>
@@ -752,10 +921,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FE52A77-9E88-B54C-829A-60F01E33428B}">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView zoomScale="125" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="B1" sqref="B1:B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -767,11 +936,8 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1">
-        <v>45.166598522649998</v>
-      </c>
       <c r="C1">
-        <f>B1/$B$20*100</f>
+        <f>remittances!E2/remittances!$E$21*100</f>
         <v>35.553162836103205</v>
       </c>
     </row>
@@ -779,11 +945,8 @@
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2">
-        <v>2.1422585671007899</v>
-      </c>
       <c r="C2">
-        <f t="shared" ref="C2:C18" si="0">B2/$B$20*100</f>
+        <f>remittances!E3/remittances!$E$21*100</f>
         <v>1.6862918653255903</v>
       </c>
     </row>
@@ -791,11 +954,8 @@
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3">
-        <v>2.1143398278595602</v>
-      </c>
       <c r="C3">
-        <f t="shared" si="0"/>
+        <f>remittances!E4/remittances!$E$21*100</f>
         <v>1.6643154598647187</v>
       </c>
     </row>
@@ -803,11 +963,8 @@
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4">
-        <v>3.94235867412231</v>
-      </c>
       <c r="C4">
-        <f>B4/$B$20*100</f>
+        <f>remittances!E5/remittances!$E$21*100</f>
         <v>3.1032516169909448</v>
       </c>
     </row>
@@ -815,11 +972,8 @@
       <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B5">
-        <v>7.8301082151755299</v>
-      </c>
       <c r="C5">
-        <f t="shared" si="0"/>
+        <f>remittances!E6/remittances!$E$21*100</f>
         <v>6.1635173226259532</v>
       </c>
     </row>
@@ -827,11 +981,8 @@
       <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="B6">
-        <v>8.7274658819365794</v>
-      </c>
       <c r="C6">
-        <f t="shared" si="0"/>
+        <f>remittances!E7/remittances!$E$21*100</f>
         <v>6.8698778698471958</v>
       </c>
     </row>
@@ -839,11 +990,8 @@
       <c r="A7" t="s">
         <v>6</v>
       </c>
-      <c r="B7">
-        <v>8.4198711172140399</v>
-      </c>
       <c r="C7">
-        <f t="shared" si="0"/>
+        <f>remittances!E8/remittances!$E$21*100</f>
         <v>6.6277527792843278</v>
       </c>
     </row>
@@ -851,11 +999,8 @@
       <c r="A8" t="s">
         <v>7</v>
       </c>
-      <c r="B8">
-        <v>5.0862148338052098</v>
-      </c>
       <c r="C8">
-        <f t="shared" si="0"/>
+        <f>remittances!E9/remittances!$E$21*100</f>
         <v>4.0036449526965745</v>
       </c>
     </row>
@@ -863,11 +1008,8 @@
       <c r="A9" t="s">
         <v>8</v>
       </c>
-      <c r="B9">
-        <v>4.7786268244620604</v>
-      </c>
       <c r="C9">
-        <f t="shared" si="0"/>
+        <f>remittances!E10/remittances!$E$21*100</f>
         <v>3.761525179671696</v>
       </c>
     </row>
@@ -875,11 +1017,8 @@
       <c r="A10" t="s">
         <v>9</v>
       </c>
-      <c r="B10">
-        <v>0.67826332163080405</v>
-      </c>
       <c r="C10">
-        <f t="shared" si="0"/>
+        <f>remittances!E11/remittances!$E$21*100</f>
         <v>0.53389910040720479</v>
       </c>
     </row>
@@ -887,11 +1026,8 @@
       <c r="A11" t="s">
         <v>10</v>
       </c>
-      <c r="B11">
-        <v>8.1229291259909395</v>
-      </c>
       <c r="C11">
-        <f t="shared" si="0"/>
+        <f>remittances!E12/remittances!$E$21*100</f>
         <v>6.3940130841966534</v>
       </c>
     </row>
@@ -899,11 +1035,8 @@
       <c r="A12" t="s">
         <v>11</v>
       </c>
-      <c r="B12">
-        <v>2.3754505915439701</v>
-      </c>
       <c r="C12">
-        <f t="shared" si="0"/>
+        <f>remittances!E13/remittances!$E$21*100</f>
         <v>1.8698503861858968</v>
       </c>
     </row>
@@ -911,11 +1044,8 @@
       <c r="A13" t="s">
         <v>12</v>
       </c>
-      <c r="B13">
-        <v>1.7552700438372899</v>
-      </c>
       <c r="C13">
-        <f t="shared" si="0"/>
+        <f>remittances!E14/remittances!$E$21*100</f>
         <v>1.3816714946684843</v>
       </c>
     </row>
@@ -923,11 +1053,8 @@
       <c r="A14" t="s">
         <v>13</v>
       </c>
-      <c r="B14">
-        <v>11.1303832019158</v>
-      </c>
       <c r="C14">
-        <f t="shared" si="0"/>
+        <f>remittances!E15/remittances!$E$21*100</f>
         <v>8.7613488584378487</v>
       </c>
     </row>
@@ -935,11 +1062,8 @@
       <c r="A15" t="s">
         <v>14</v>
       </c>
-      <c r="B15">
-        <v>0.79759144842393304</v>
-      </c>
       <c r="C15">
-        <f t="shared" si="0"/>
+        <f>remittances!E16/remittances!$E$21*100</f>
         <v>0.62782896144546241</v>
       </c>
     </row>
@@ -947,11 +1071,8 @@
       <c r="A16" t="s">
         <v>15</v>
       </c>
-      <c r="B16">
-        <v>5.5518454757455604</v>
-      </c>
       <c r="C16">
-        <f t="shared" si="0"/>
+        <f>remittances!E17/remittances!$E$21*100</f>
         <v>4.3701689455556512</v>
       </c>
     </row>
@@ -959,11 +1080,8 @@
       <c r="A17" t="s">
         <v>16</v>
       </c>
-      <c r="B17">
-        <v>1.65591512835032</v>
-      </c>
       <c r="C17">
-        <f t="shared" si="0"/>
+        <f>remittances!E18/remittances!$E$21*100</f>
         <v>1.3034636684337035</v>
       </c>
     </row>
@@ -971,18 +1089,9 @@
       <c r="A18" t="s">
         <v>17</v>
       </c>
-      <c r="B18">
-        <v>6.7641167033786296</v>
-      </c>
       <c r="C18">
-        <f t="shared" si="0"/>
+        <f>remittances!E19/remittances!$E$21*100</f>
         <v>5.324415618258878</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B20">
-        <f>SUM(B1:B18)</f>
-        <v>127.03960750514334</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
edited narrative of remit
</commit_message>
<xml_diff>
--- a/data/avg_spending_byCat_normalized.xlsx
+++ b/data/avg_spending_byCat_normalized.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/runlanlana/Documents/2023_Spring/MIT6.C85_Interactive Data Visualization and Society/Final Project/MigrationMDT/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07E8CBD2-3E7E-2043-AF58-2F30CBD495F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4147A870-EF43-314B-B7C5-3D3EB98EAD05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1180" yWindow="1500" windowWidth="27240" windowHeight="15380" xr2:uid="{90FB2B7F-F2DC-A947-B420-8E21EAE8B889}"/>
   </bookViews>
@@ -17,6 +17,9 @@
     <sheet name="No remittances" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">remittances!$A$1:$F$1</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -476,19 +479,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44DB7E41-2D86-5346-BF0E-2692AD0D4BF7}">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="135" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="31.33203125" customWidth="1"/>
     <col min="4" max="4" width="22.6640625" customWidth="1"/>
+    <col min="6" max="6" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>23</v>
       </c>
@@ -508,29 +512,37 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="C2">
-        <v>69.3057958002764</v>
+        <v>2.6742174037088202</v>
       </c>
       <c r="D2">
         <f>C2/$C$21*100</f>
-        <v>33.772619365877986</v>
+        <v>1.3031424779730223</v>
       </c>
       <c r="E2">
-        <v>45.166598522649998</v>
+        <v>1.7552700438372899</v>
       </c>
       <c r="F2">
         <f>E2/C2</f>
-        <v>0.65170016448277868</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+        <v>0.65636774385019703</v>
+      </c>
+      <c r="G2">
+        <f>C2/E2-1</f>
+        <v>0.52353617216788484</v>
+      </c>
+      <c r="H2">
+        <f>1-E2/C2</f>
+        <v>0.34363225614980297</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -541,84 +553,116 @@
         <v>3.83894286454733</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D19" si="0">C3/$C$21*100</f>
-        <v>1.8707115997244377</v>
+        <f>C3/$C$21*100</f>
+        <v>1.8707115997244381</v>
       </c>
       <c r="E3">
         <v>2.1422585671007899</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F19" si="1">E3/C3</f>
+        <f>E3/C3</f>
         <v>0.55803345938918913</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G3">
+        <f t="shared" ref="G3:G19" si="0">C3/E3-1</f>
+        <v>0.7920072410972947</v>
+      </c>
+      <c r="H3">
+        <f t="shared" ref="H3:H19" si="1">1-E3/C3</f>
+        <v>0.44196654061081087</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C4">
-        <v>3.7083922736696602</v>
+        <v>69.3057958002764</v>
       </c>
       <c r="D4">
-        <f t="shared" si="0"/>
-        <v>1.8070944756038538</v>
+        <f>C4/$C$21*100</f>
+        <v>33.772619365877993</v>
       </c>
       <c r="E4">
-        <v>2.1143398278595602</v>
+        <v>45.166598522649998</v>
       </c>
       <c r="F4">
-        <f t="shared" si="1"/>
-        <v>0.57014999272644462</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+        <f>E4/C4</f>
+        <v>0.65170016448277868</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="0"/>
+        <v>0.53444797853265746</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="1"/>
+        <v>0.34829983551722132</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5">
+        <v>20.2649104235199</v>
+      </c>
+      <c r="D5">
+        <f>C5/$C$21*100</f>
+        <v>9.8750630926947878</v>
+      </c>
+      <c r="E5">
+        <v>8.1229291259909395</v>
+      </c>
+      <c r="F5">
+        <f>E5/C5</f>
+        <v>0.40083715921898622</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="0"/>
+        <v>1.4947786825663982</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="1"/>
+        <v>0.59916284078101378</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>19</v>
       </c>
-      <c r="B5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5">
-        <v>4.9770539813407</v>
-      </c>
-      <c r="D5">
-        <f t="shared" si="0"/>
-        <v>2.4253115880761116</v>
-      </c>
-      <c r="E5">
-        <v>3.94235867412231</v>
-      </c>
-      <c r="F5">
-        <f t="shared" si="1"/>
-        <v>0.79210687464963603</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>18</v>
-      </c>
       <c r="B6" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="C6">
-        <v>12.323934897719401</v>
+        <v>18.550576412117</v>
       </c>
       <c r="D6">
-        <f t="shared" si="0"/>
-        <v>6.0054365956631566</v>
+        <f>C6/$C$21*100</f>
+        <v>9.0396704770478014</v>
       </c>
       <c r="E6">
-        <v>7.8301082151755299</v>
+        <v>6.7641167033786296</v>
       </c>
       <c r="F6">
-        <f t="shared" si="1"/>
-        <v>0.63535780415592158</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+        <f>E6/C6</f>
+        <v>0.36463107954750101</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="0"/>
+        <v>1.7424979824566176</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="1"/>
+        <v>0.63536892045249904</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -629,292 +673,408 @@
         <v>13.355644344851401</v>
       </c>
       <c r="D7">
-        <f t="shared" si="0"/>
+        <f>C7/$C$21*100</f>
         <v>6.5081871961263653</v>
       </c>
       <c r="E7">
         <v>8.7274658819365794</v>
       </c>
       <c r="F7">
-        <f t="shared" si="1"/>
+        <f>E7/C7</f>
         <v>0.65346647878512998</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G7">
+        <f t="shared" si="0"/>
+        <v>0.53030037877247516</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="1"/>
+        <v>0.34653352121487002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B8" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C8">
-        <v>11.050803309606</v>
+        <v>4.9770539813407</v>
       </c>
       <c r="D8">
-        <f t="shared" si="0"/>
-        <v>5.3850413165736954</v>
+        <f>C8/$C$21*100</f>
+        <v>2.425311588076112</v>
       </c>
       <c r="E8">
-        <v>8.4198711172140399</v>
+        <v>3.94235867412231</v>
       </c>
       <c r="F8">
-        <f t="shared" si="1"/>
-        <v>0.76192389650940573</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+        <f>E8/C8</f>
+        <v>0.79210687464963603</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="0"/>
+        <v>0.26245590336824054</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="1"/>
+        <v>0.20789312535036397</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B9" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C9">
-        <v>7.9561684429854802</v>
+        <v>2.6107303132918598</v>
       </c>
       <c r="D9">
-        <f t="shared" si="0"/>
-        <v>3.8770299847662546</v>
+        <f>C9/$C$21*100</f>
+        <v>1.2722053057705998</v>
       </c>
       <c r="E9">
-        <v>5.0862148338052098</v>
+        <v>0.79759144842393304</v>
       </c>
       <c r="F9">
-        <f t="shared" si="1"/>
-        <v>0.63927943082822081</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+        <f>E9/C9</f>
+        <v>0.30550510880545645</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="0"/>
+        <v>2.2732676841643036</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="1"/>
+        <v>0.69449489119454355</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B10" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C10">
-        <v>6.51870951071181</v>
+        <v>1.4913128997926699</v>
       </c>
       <c r="D10">
-        <f t="shared" si="0"/>
-        <v>3.1765582159453492</v>
+        <f>C10/$C$21*100</f>
+        <v>0.72671473342956305</v>
       </c>
       <c r="E10">
-        <v>4.7786268244620604</v>
+        <v>0.67826332163080405</v>
       </c>
       <c r="F10">
-        <f t="shared" si="1"/>
-        <v>0.73306331822420145</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+        <f>E10/C10</f>
+        <v>0.45480953173884553</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>1.1987226085098985</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="1"/>
+        <v>0.54519046826115447</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>20</v>
       </c>
       <c r="B11" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C11">
-        <v>1.4913128997926699</v>
+        <v>3.19143003109882</v>
       </c>
       <c r="D11">
-        <f t="shared" si="0"/>
-        <v>0.72671473342956294</v>
+        <f>C11/$C$21*100</f>
+        <v>1.5551794828781516</v>
       </c>
       <c r="E11">
-        <v>0.67826332163080405</v>
+        <v>2.3754505915439701</v>
       </c>
       <c r="F11">
-        <f t="shared" si="1"/>
-        <v>0.45480953173884553</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+        <f>E11/C11</f>
+        <v>0.74432168914763719</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="0"/>
+        <v>0.34350511960111452</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="1"/>
+        <v>0.25567831085236281</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="B12" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C12">
-        <v>20.2649104235199</v>
+        <v>5.5735141258926504</v>
       </c>
       <c r="D12">
-        <f t="shared" si="0"/>
-        <v>9.8750630926947878</v>
+        <f>C12/$C$21*100</f>
+        <v>2.7159657995495667</v>
       </c>
       <c r="E12">
-        <v>8.1229291259909395</v>
+        <v>5.5518454757455604</v>
       </c>
       <c r="F12">
-        <f t="shared" si="1"/>
-        <v>0.40083715921898622</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+        <f>E12/C12</f>
+        <v>0.99611221041919951</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="0"/>
+        <v>3.9029634815583858E-3</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="1"/>
+        <v>3.8877895808004936E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B13" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C13">
-        <v>3.19143003109882</v>
+        <v>4.8390416220916803</v>
       </c>
       <c r="D13">
-        <f t="shared" si="0"/>
-        <v>1.5551794828781513</v>
+        <f>C13/$C$21*100</f>
+        <v>2.3580583544484943</v>
       </c>
       <c r="E13">
-        <v>2.3754505915439701</v>
+        <v>1.65591512835032</v>
       </c>
       <c r="F13">
-        <f t="shared" si="1"/>
-        <v>0.74432168914763719</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+        <f>E13/C13</f>
+        <v>0.34219898435892127</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="0"/>
+        <v>1.9222763529629088</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="1"/>
+        <v>0.65780101564107873</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="B14" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C14">
-        <v>2.6742174037088202</v>
+        <v>12.981792979497801</v>
       </c>
       <c r="D14">
-        <f t="shared" si="0"/>
-        <v>1.3031424779730221</v>
+        <f>C14/$C$21*100</f>
+        <v>6.3260099378507944</v>
       </c>
       <c r="E14">
-        <v>1.7552700438372899</v>
+        <v>11.1303832019158</v>
       </c>
       <c r="F14">
-        <f t="shared" si="1"/>
-        <v>0.65636774385019703</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+        <f>E14/C14</f>
+        <v>0.85738412401846653</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="0"/>
+        <v>0.16633836805037672</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="1"/>
+        <v>0.14261587598153347</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="B15" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C15">
-        <v>12.981792979497801</v>
+        <v>11.050803309606</v>
       </c>
       <c r="D15">
-        <f t="shared" si="0"/>
-        <v>6.3260099378507935</v>
+        <f>C15/$C$21*100</f>
+        <v>5.3850413165736963</v>
       </c>
       <c r="E15">
-        <v>11.1303832019158</v>
+        <v>8.4198711172140399</v>
       </c>
       <c r="F15">
-        <f t="shared" si="1"/>
-        <v>0.85738412401846653</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+        <f>E15/C15</f>
+        <v>0.76192389650940573</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="0"/>
+        <v>0.31246703848152024</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="1"/>
+        <v>0.23807610349059427</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B16" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="C16">
-        <v>2.6107303132918598</v>
+        <v>3.7083922736696602</v>
       </c>
       <c r="D16">
-        <f t="shared" si="0"/>
-        <v>1.2722053057705995</v>
+        <f>C16/$C$21*100</f>
+        <v>1.8070944756038543</v>
       </c>
       <c r="E16">
-        <v>0.79759144842393304</v>
+        <v>2.1143398278595602</v>
       </c>
       <c r="F16">
-        <f t="shared" si="1"/>
-        <v>0.30550510880545645</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+        <f>E16/C16</f>
+        <v>0.57014999272644462</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="0"/>
+        <v>0.75392442823338857</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="1"/>
+        <v>0.42985000727355538</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B17" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="C17">
-        <v>5.5735141258926504</v>
+        <v>12.323934897719401</v>
       </c>
       <c r="D17">
-        <f t="shared" si="0"/>
-        <v>2.7159657995495663</v>
+        <f>C17/$C$21*100</f>
+        <v>6.0054365956631575</v>
       </c>
       <c r="E17">
-        <v>5.5518454757455604</v>
+        <v>7.8301082151755299</v>
       </c>
       <c r="F17">
-        <f t="shared" si="1"/>
-        <v>0.99611221041919951</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+        <f>E17/C17</f>
+        <v>0.63535780415592158</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="0"/>
+        <v>0.57391629324284255</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="1"/>
+        <v>0.36464219584407842</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="C18">
-        <v>4.8390416220916803</v>
+        <v>7.9561684429854802</v>
       </c>
       <c r="D18">
-        <f t="shared" si="0"/>
-        <v>2.3580583544484943</v>
+        <f>C18/$C$21*100</f>
+        <v>3.877029984766255</v>
       </c>
       <c r="E18">
-        <v>1.65591512835032</v>
+        <v>5.0862148338052098</v>
       </c>
       <c r="F18">
-        <f t="shared" si="1"/>
-        <v>0.34219898435892127</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+        <f>E18/C18</f>
+        <v>0.63927943082822081</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="0"/>
+        <v>0.56426118497891653</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="1"/>
+        <v>0.36072056917177919</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="C19">
-        <v>18.550576412117</v>
+        <v>6.51870951071181</v>
       </c>
       <c r="D19">
-        <f t="shared" si="0"/>
-        <v>9.0396704770477996</v>
+        <f>C19/$C$21*100</f>
+        <v>3.17655821594535</v>
       </c>
       <c r="E19">
-        <v>6.7641167033786296</v>
+        <v>4.7786268244620604</v>
       </c>
       <c r="F19">
-        <f t="shared" si="1"/>
-        <v>0.36463107954750101</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+        <f>E19/C19</f>
+        <v>0.73306331822420145</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="0"/>
+        <v>0.36413864278795915</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="1"/>
+        <v>0.26693668177579855</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C21">
         <f>SUM(C2:C19)</f>
-        <v>205.2129716367194</v>
+        <v>205.21297163671937</v>
       </c>
       <c r="E21">
         <f>SUM(E2:E19)</f>
-        <v>127.03960750514334</v>
+        <v>127.03960750514335</v>
+      </c>
+      <c r="G21">
+        <f>C21/E21-1</f>
+        <v>0.61534639209595388</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:F1" xr:uid="{44DB7E41-2D86-5346-BF0E-2692AD0D4BF7}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F19">
+      <sortCondition descending="1" ref="A1:A19"/>
+    </sortState>
+  </autoFilter>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F19">
+    <sortCondition ref="A4:A19"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -938,7 +1098,7 @@
       </c>
       <c r="C1">
         <f>remittances!E2/remittances!$E$21*100</f>
-        <v>35.553162836103205</v>
+        <v>1.381671494668484</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -947,7 +1107,7 @@
       </c>
       <c r="C2">
         <f>remittances!E3/remittances!$E$21*100</f>
-        <v>1.6862918653255903</v>
+        <v>1.6862918653255898</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -956,7 +1116,7 @@
       </c>
       <c r="C3">
         <f>remittances!E4/remittances!$E$21*100</f>
-        <v>1.6643154598647187</v>
+        <v>35.553162836103205</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -965,7 +1125,7 @@
       </c>
       <c r="C4">
         <f>remittances!E5/remittances!$E$21*100</f>
-        <v>3.1032516169909448</v>
+        <v>6.3940130841966534</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -974,7 +1134,7 @@
       </c>
       <c r="C5">
         <f>remittances!E6/remittances!$E$21*100</f>
-        <v>6.1635173226259532</v>
+        <v>5.3244156182588771</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -983,7 +1143,7 @@
       </c>
       <c r="C6">
         <f>remittances!E7/remittances!$E$21*100</f>
-        <v>6.8698778698471958</v>
+        <v>6.869877869847195</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -992,7 +1152,7 @@
       </c>
       <c r="C7">
         <f>remittances!E8/remittances!$E$21*100</f>
-        <v>6.6277527792843278</v>
+        <v>3.1032516169909443</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -1001,7 +1161,7 @@
       </c>
       <c r="C8">
         <f>remittances!E9/remittances!$E$21*100</f>
-        <v>4.0036449526965745</v>
+        <v>0.6278289614454623</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -1010,7 +1170,7 @@
       </c>
       <c r="C9">
         <f>remittances!E10/remittances!$E$21*100</f>
-        <v>3.761525179671696</v>
+        <v>0.53389910040720467</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -1019,7 +1179,7 @@
       </c>
       <c r="C10">
         <f>remittances!E11/remittances!$E$21*100</f>
-        <v>0.53389910040720479</v>
+        <v>1.8698503861858964</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -1028,7 +1188,7 @@
       </c>
       <c r="C11">
         <f>remittances!E12/remittances!$E$21*100</f>
-        <v>6.3940130841966534</v>
+        <v>4.3701689455556503</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -1037,7 +1197,7 @@
       </c>
       <c r="C12">
         <f>remittances!E13/remittances!$E$21*100</f>
-        <v>1.8698503861858968</v>
+        <v>1.3034636684337033</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -1046,7 +1206,7 @@
       </c>
       <c r="C13">
         <f>remittances!E14/remittances!$E$21*100</f>
-        <v>1.3816714946684843</v>
+        <v>8.7613488584378487</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -1055,7 +1215,7 @@
       </c>
       <c r="C14">
         <f>remittances!E15/remittances!$E$21*100</f>
-        <v>8.7613488584378487</v>
+        <v>6.6277527792843278</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -1064,7 +1224,7 @@
       </c>
       <c r="C15">
         <f>remittances!E16/remittances!$E$21*100</f>
-        <v>0.62782896144546241</v>
+        <v>1.6643154598647187</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
@@ -1073,7 +1233,7 @@
       </c>
       <c r="C16">
         <f>remittances!E17/remittances!$E$21*100</f>
-        <v>4.3701689455556512</v>
+        <v>6.1635173226259523</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -1082,7 +1242,7 @@
       </c>
       <c r="C17">
         <f>remittances!E18/remittances!$E$21*100</f>
-        <v>1.3034636684337035</v>
+        <v>4.0036449526965736</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -1091,7 +1251,7 @@
       </c>
       <c r="C18">
         <f>remittances!E19/remittances!$E$21*100</f>
-        <v>5.324415618258878</v>
+        <v>3.761525179671696</v>
       </c>
     </row>
   </sheetData>

</xml_diff>